<commit_message>
Unit Test Shenanigans part 2
</commit_message>
<xml_diff>
--- a/UnitTest CheatSheat.xlsx
+++ b/UnitTest CheatSheat.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Práce\GitHub\ROP-HashTester\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Ročníková Práce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F4168A-A73E-42F5-A3A2-EE05568F7080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCBDDC9-4ECA-49E0-9A7E-BFAD4C93213D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="98">
   <si>
     <t>String</t>
   </si>
@@ -136,13 +136,196 @@
   </si>
   <si>
     <t>GRADUAL HASHING</t>
+  </si>
+  <si>
+    <t>Testus</t>
+  </si>
+  <si>
+    <t>b9ece18c950afbfa6b0fdbfa4ff731d3</t>
+  </si>
+  <si>
+    <t>2408730ad248ad4e4aa36fb14f5e0631</t>
+  </si>
+  <si>
+    <t>78ac12266411beaf4149f5cfb6e33afd</t>
+  </si>
+  <si>
+    <t>0cbc6611f5540bd0809a388dc95a615b</t>
+  </si>
+  <si>
+    <t>4e73c38e86323e3f00a309e6bcdcea46</t>
+  </si>
+  <si>
+    <t>021034f85e1577648504c45f70486e2c</t>
+  </si>
+  <si>
+    <t>c2c53d66948214258a26ca9ca845d7ac0c17f8e7</t>
+  </si>
+  <si>
+    <t>1b1be06f5bfb451c3199aeb9e8e337905dd0cecb</t>
+  </si>
+  <si>
+    <t>c82524e086d9a253cce031af2342715692b79aac</t>
+  </si>
+  <si>
+    <t>640ab2bae07bedc4c163f679a746f7ab7fb5d1fa</t>
+  </si>
+  <si>
+    <t>2d3d360a82c6464020c5cd02b2352b74c8b6df6f</t>
+  </si>
+  <si>
+    <t>9d4b621d6602beb27e1fb82dbeb841dd7897661d</t>
+  </si>
+  <si>
+    <t>e632b7095b0bf32c260fa4c539e9fd7b852d0de454e9be26f24d0d6f91d069d3</t>
+  </si>
+  <si>
+    <t>7566ad8da86a586045385d1bdc1f1f26df9257280bf47a5c2975ee926dee3e6e</t>
+  </si>
+  <si>
+    <t>47e8f094e1aca27195e6de64d47e8aa2b4f9c234d95da517084e0926fdaa8ba1</t>
+  </si>
+  <si>
+    <t>532eaabd9574880dbf76b9b8cc00832c20a6ec113d682299550d7a6e0f345e25</t>
+  </si>
+  <si>
+    <t>e835808c8a4b7b3e5c1fa276b121c382f74755a7c0dae908867209ef67fbce8b</t>
+  </si>
+  <si>
+    <t>ca21ae9392cb39a8eddd8d76a33735e779a909aada3b66ccfa71fa8a22052f38</t>
+  </si>
+  <si>
+    <t>b2396a002fe7aec008808687d7cbacb340b7f7a090008382f3c95870f6fb10415f61f5737c102d4bfec58fe525407ea2001e761dab1da8a501d9523921f0ec21</t>
+  </si>
+  <si>
+    <t>cc12409c9f6cb05f7b8b959fcf5454ba457fccbf9fc83b278850a524b4962ee1ff81810f7ddb86fd16601c22548e3809dc440afd2701702268fcb91907fcff53</t>
+  </si>
+  <si>
+    <t>71a0ec8b3318b49a9f5a12205a9cdedc9ac6b01a447c8b21c824aa33da564f1864a65476f03d1de71d12ea294555c810f9f9da8326c4ad13f151aa3ba7a33fd5</t>
+  </si>
+  <si>
+    <t>c6ee9e33cf5c6715a1d148fd73f7318884b41adcb916021e2bc0e800a5c5dd97f5142178f6ae88c8fdd98e1afb0ce4c8d2c54b5f37b30b7da1997bb33b0b8a31</t>
+  </si>
+  <si>
+    <t>726a250d106f6636303b67ee16fc2852bc28fb7c61cdc8b8c8da349a263fd2384cdb6e72e08cf62aa573b6a205483806180b57c3430b90bb8819738994e9306c</t>
+  </si>
+  <si>
+    <t>6db16199111b65d307e5af1575a0e97dfecde1705a056dc92feb6e0b29444241996556d48359e7c59a369158462d4d0b151545667f701d365c45914cd8029f3c</t>
+  </si>
+  <si>
+    <t>9de1976650ec90e603d2892e43015af720d91fe4</t>
+  </si>
+  <si>
+    <t>77503acf53f822816d66efcf47be6a05027b495f</t>
+  </si>
+  <si>
+    <t>dcbc4a87d4df24b0b640a91ffa15b83888ffe492</t>
+  </si>
+  <si>
+    <t>76c82682cd7af7e812e513fa0e7914ab40b842e0</t>
+  </si>
+  <si>
+    <t>a3b588877caf94021b02759a35b0684b30235221</t>
+  </si>
+  <si>
+    <t>1460cbcc6d2447d17044b8d003d0b669fe999365</t>
+  </si>
+  <si>
+    <t>be047a60</t>
+  </si>
+  <si>
+    <t>a2d61f78</t>
+  </si>
+  <si>
+    <t>4572e01a</t>
+  </si>
+  <si>
+    <t>784dd132</t>
+  </si>
+  <si>
+    <t>3ac2766f</t>
+  </si>
+  <si>
+    <t>c63971b4</t>
+  </si>
+  <si>
+    <t>Salt</t>
+  </si>
+  <si>
+    <t>Pepper</t>
+  </si>
+  <si>
+    <t>HASHER SALT PEPPER</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>salt101</t>
+  </si>
+  <si>
+    <t>M5</t>
+  </si>
+  <si>
+    <t>b9f2d25febd39790a6a6b3163c672ec6</t>
+  </si>
+  <si>
+    <t>a1ccf36317c6cf2d98bc03832ee35499e3dc62fe</t>
+  </si>
+  <si>
+    <t>ad853ef97f34098a94f3f1ab59c6301c334ccc7b0c1ebfc2f6c5eb6bff60078d</t>
+  </si>
+  <si>
+    <t>75a8914a2a4aeabea4cf8e1fef4d255f63708c96f118543cd0ef54db056d7b4f1ea9df4d0365119866c8ab8a85fcd45155b8108fb9c48e90074dbc8f5d19dd3a</t>
+  </si>
+  <si>
+    <t>1a85bcb6</t>
+  </si>
+  <si>
+    <t>7cef35065a9df17b8222781a616052cf6199c1b9</t>
+  </si>
+  <si>
+    <t>d4a38bab94c4341032fd5109452635dc</t>
+  </si>
+  <si>
+    <t>e9cdf0941adf6a4c11b29fec31b63210e2d79b29</t>
+  </si>
+  <si>
+    <t>b9e79e9e860692da02b7a6e3cc0fd30f8d0bdbe185c0dbc5cdcd78e8514e176b</t>
+  </si>
+  <si>
+    <t>3c3bf36c33157d048629df3483be44853d14514989db0c6d0b8eb38a73f927833b01a55d48a40806f2c7c628bf88347cc2c99b778154c29b318973793b4088a8</t>
+  </si>
+  <si>
+    <t>3f75d493</t>
+  </si>
+  <si>
+    <t>4e4aa21551256fddc151d31719cec0bade0f5b9c</t>
+  </si>
+  <si>
+    <t>ffd60eb4265b259bd41cf1ecf9168d65</t>
+  </si>
+  <si>
+    <t>610966b737670c4957cefa62884cbda5d06b6e94</t>
+  </si>
+  <si>
+    <t>0967200e8d4e27894d2bf53d318a3efe2efada1de1c13dc910ef9558592e3858</t>
+  </si>
+  <si>
+    <t>56af63202c76821d777a1aa088444098e8ff87f18cc36efdda5803cc7331ac0ed1c3d7daaf4c5465620f625d3f5a31c263c07b9c6bc15c9e48c8bea83558ac59</t>
+  </si>
+  <si>
+    <t>22f50b88</t>
+  </si>
+  <si>
+    <t>001bc637637344af6f63ca9ecf2cfe0fdbff8ba4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +353,15 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -191,11 +383,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -476,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,133 +680,345 @@
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>24</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>28</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C3" s="3">
         <v>1234567890</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>25</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>29</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>30</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>23</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>27</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>31</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" t="s">
+        <v>64</v>
+      </c>
+      <c r="J9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" t="s">
+        <v>66</v>
+      </c>
+      <c r="J11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" t="s">
+        <v>83</v>
+      </c>
+      <c r="I14" t="s">
+        <v>85</v>
+      </c>
+      <c r="J14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" t="s">
+        <v>87</v>
+      </c>
+      <c r="G15" t="s">
+        <v>88</v>
+      </c>
+      <c r="H15" t="s">
+        <v>89</v>
+      </c>
+      <c r="I15" t="s">
+        <v>91</v>
+      </c>
+      <c r="J15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16" t="s">
+        <v>93</v>
+      </c>
+      <c r="G16" t="s">
+        <v>94</v>
+      </c>
+      <c r="H16" t="s">
+        <v>95</v>
+      </c>
+      <c r="I16" t="s">
+        <v>97</v>
+      </c>
+      <c r="J16" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>